<commit_message>
finished tax_rate plots in matplotlib
</commit_message>
<xml_diff>
--- a/progressivity_pres/payoffs_table.xlsx
+++ b/progressivity_pres/payoffs_table.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,6 +453,21 @@
       <c r="G1" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -464,18 +479,33 @@
         <v>45</v>
       </c>
       <c r="C2" t="n">
+        <v>59.528</v>
+      </c>
+      <c r="D2" t="n">
         <v>71.88</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
+        <v>83.89700000000001</v>
+      </c>
+      <c r="F2" t="n">
         <v>98.053</v>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
+        <v>114.98</v>
+      </c>
+      <c r="H2" t="n">
         <v>115.604</v>
       </c>
-      <c r="F2" t="n">
+      <c r="I2" t="n">
+        <v>100.304</v>
+      </c>
+      <c r="J2" t="n">
         <v>85.004</v>
       </c>
-      <c r="G2" t="n">
+      <c r="K2" t="n">
+        <v>69.70399999999999</v>
+      </c>
+      <c r="L2" t="n">
         <v>54.404</v>
       </c>
     </row>
@@ -489,18 +519,33 @@
         <v>75</v>
       </c>
       <c r="C3" t="n">
+        <v>98.307</v>
+      </c>
+      <c r="D3" t="n">
         <v>116.82</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
+        <v>132.38</v>
+      </c>
+      <c r="F3" t="n">
         <v>147.463</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
+        <v>162.699</v>
+      </c>
+      <c r="H3" t="n">
         <v>156.404</v>
       </c>
-      <c r="F3" t="n">
+      <c r="I3" t="n">
+        <v>130.904</v>
+      </c>
+      <c r="J3" t="n">
         <v>105.404</v>
       </c>
-      <c r="G3" t="n">
+      <c r="K3" t="n">
+        <v>79.904</v>
+      </c>
+      <c r="L3" t="n">
         <v>54.404</v>
       </c>
     </row>
@@ -514,18 +559,33 @@
         <v>125</v>
       </c>
       <c r="C4" t="n">
+        <v>162.938</v>
+      </c>
+      <c r="D4" t="n">
         <v>191.72</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
+        <v>213.187</v>
+      </c>
+      <c r="F4" t="n">
         <v>229.813</v>
       </c>
-      <c r="E4" t="n">
+      <c r="G4" t="n">
+        <v>242.23</v>
+      </c>
+      <c r="H4" t="n">
         <v>224.404</v>
       </c>
-      <c r="F4" t="n">
+      <c r="I4" t="n">
+        <v>181.904</v>
+      </c>
+      <c r="J4" t="n">
         <v>139.404</v>
       </c>
-      <c r="G4" t="n">
+      <c r="K4" t="n">
+        <v>96.904</v>
+      </c>
+      <c r="L4" t="n">
         <v>54.404</v>
       </c>
     </row>
@@ -539,18 +599,33 @@
         <v>200</v>
       </c>
       <c r="C5" t="n">
+        <v>259.885</v>
+      </c>
+      <c r="D5" t="n">
         <v>304.07</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
+        <v>334.396</v>
+      </c>
+      <c r="F5" t="n">
         <v>353.338</v>
       </c>
-      <c r="E5" t="n">
+      <c r="G5" t="n">
+        <v>361.527</v>
+      </c>
+      <c r="H5" t="n">
         <v>326.404</v>
       </c>
-      <c r="F5" t="n">
+      <c r="I5" t="n">
+        <v>258.404</v>
+      </c>
+      <c r="J5" t="n">
         <v>190.404</v>
       </c>
-      <c r="G5" t="n">
+      <c r="K5" t="n">
+        <v>122.404</v>
+      </c>
+      <c r="L5" t="n">
         <v>54.404</v>
       </c>
     </row>
@@ -564,18 +639,33 @@
         <v>400</v>
       </c>
       <c r="C6" t="n">
+        <v>518.41</v>
+      </c>
+      <c r="D6" t="n">
         <v>603.67</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
+        <v>657.621</v>
+      </c>
+      <c r="F6" t="n">
         <v>682.7380000000001</v>
       </c>
-      <c r="E6" t="n">
+      <c r="G6" t="n">
+        <v>679.652</v>
+      </c>
+      <c r="H6" t="n">
         <v>598.404</v>
       </c>
-      <c r="F6" t="n">
+      <c r="I6" t="n">
+        <v>462.404</v>
+      </c>
+      <c r="J6" t="n">
         <v>326.404</v>
       </c>
-      <c r="G6" t="n">
+      <c r="K6" t="n">
+        <v>190.404</v>
+      </c>
+      <c r="L6" t="n">
         <v>54.404</v>
       </c>
     </row>
@@ -589,18 +679,33 @@
         <v>625</v>
       </c>
       <c r="C7" t="n">
+        <v>809.251</v>
+      </c>
+      <c r="D7" t="n">
         <v>940.72</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
+        <v>1021.249</v>
+      </c>
+      <c r="F7" t="n">
         <v>1053.313</v>
       </c>
-      <c r="E7" t="n">
+      <c r="G7" t="n">
+        <v>1037.543</v>
+      </c>
+      <c r="H7" t="n">
         <v>904.404</v>
       </c>
-      <c r="F7" t="n">
+      <c r="I7" t="n">
+        <v>691.904</v>
+      </c>
+      <c r="J7" t="n">
         <v>479.404</v>
       </c>
-      <c r="G7" t="n">
+      <c r="K7" t="n">
+        <v>266.904</v>
+      </c>
+      <c r="L7" t="n">
         <v>54.404</v>
       </c>
     </row>

</xml_diff>